<commit_message>
feat: init MVP! it works
</commit_message>
<xml_diff>
--- a/input/TICKER_TEMPLATE.xlsx
+++ b/input/TICKER_TEMPLATE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvuolo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvuolo/Documents/GitHub/dca-2k24/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963818CA-0F52-5D41-8E9C-F8980FD3C67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA72F4B-439B-A041-A094-86840CD45F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7620" yWindow="500" windowWidth="40860" windowHeight="28300" activeTab="6" xr2:uid="{372CD787-09C0-4BD9-A6AB-A0065DACB93A}"/>
   </bookViews>
@@ -1813,16 +1813,16 @@
     <t>2021</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
+    <t>Date 1</t>
+  </si>
+  <si>
+    <t>Date 4</t>
+  </si>
+  <si>
+    <t>Date 3</t>
+  </si>
+  <si>
+    <t>Date 2</t>
   </si>
 </sst>
 </file>
@@ -1953,7 +1953,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -2372,6 +2372,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2379,7 +2501,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2552,10 +2674,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -2568,41 +2686,42 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2610,256 +2729,206 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="75">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF006100"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF006100"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="none"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2983,6 +3052,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2998,26 +3077,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3053,451 +3112,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3682,6 +3301,256 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -3951,7 +3820,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{253B711E-A697-4B4C-A068-D1C08A843005}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowBorderDxfId="83" tableBorderDxfId="82" totalsRowBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{253B711E-A697-4B4C-A068-D1C08A843005}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowBorderDxfId="74" tableBorderDxfId="73" totalsRowBorderDxfId="72">
   <autoFilter ref="A1:F11" xr:uid="{253B711E-A697-4B4C-A068-D1C08A843005}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3961,42 +3830,28 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7AB49245-51F1-4070-A86C-81CE45F495CE}" name="stock" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{B4E0321D-4B44-4919-BCB4-EF621D867055}" name="dca score" dataDxfId="79" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{7BFE9E84-273B-41D7-A976-4742ED35CB71}" name="old price (feb 22/2022)" dataDxfId="78" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{49C5BB08-4E50-4DC3-B9E5-7D867F49F5CE}" name="current price (sept 6/2024)" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{C5CFD8CB-0AF8-4123-9315-ABDE54AD3CD9}" name="% change" dataDxfId="76" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{7AB49245-51F1-4070-A86C-81CE45F495CE}" name="stock" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{B4E0321D-4B44-4919-BCB4-EF621D867055}" name="dca score" dataDxfId="70" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{7BFE9E84-273B-41D7-A976-4742ED35CB71}" name="old price (feb 22/2022)" dataDxfId="69" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{49C5BB08-4E50-4DC3-B9E5-7D867F49F5CE}" name="current price (sept 6/2024)" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{C5CFD8CB-0AF8-4123-9315-ABDE54AD3CD9}" name="% change" dataDxfId="67" dataCellStyle="Percent">
       <calculatedColumnFormula>(D2-C2)/C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0AB9C9C3-A4A0-499B-8968-F6E512DCBD7E}" name="s&amp;p 500 % change" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{0AB9C9C3-A4A0-499B-8968-F6E512DCBD7E}" name="s&amp;p 500 % change" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4E6381B4-381E-154C-8775-3671B47E4E5C}" name="StockScores4" displayName="StockScores4" ref="B2:F17" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AF8B2C58-037A-4247-A0BE-AF3EA9857699}" name="StockScores" displayName="StockScores" ref="B2:F17" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" dataCellStyle="Comma">
   <autoFilter ref="B2:F17" xr:uid="{AF8B2C58-037A-4247-A0BE-AF3EA9857699}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1985284E-47BD-2440-BC23-6DF62CD04089}" name="Balance Sheet" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{3DBCDAFF-AA77-C342-819D-8BB1FB108DEB}" name="Column1" dataDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{DBE2CD41-0D84-4845-BE1B-D9C7F060C507}" name="Column2" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{BA158CEE-76FB-674B-8F5A-720A89298FA2}" name="Column3" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{20C06679-560B-A440-BA99-BF5FA277971F}" name="Column4" dataDxfId="0" dataCellStyle="Comma"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AF8B2C58-037A-4247-A0BE-AF3EA9857699}" name="StockScores" displayName="StockScores" ref="B2:F17" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" headerRowBorderDxfId="37" tableBorderDxfId="36" dataCellStyle="Comma">
-  <autoFilter ref="B2:F17" xr:uid="{AF8B2C58-037A-4247-A0BE-AF3EA9857699}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1B444E7A-FFC9-6B49-91BB-1031C0708A5E}" name="Balance Sheet" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{D3F71987-10EB-C24C-A913-E3218D5AFC35}" name="2024" dataDxfId="34" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{72BC2940-218A-304A-AAD0-A2F5E78D3BBC}" name="2023" dataDxfId="33" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{86C26E68-D535-F24E-9210-117B8E1D52B4}" name="2022" dataDxfId="32" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{0E7F4F14-D42E-7647-9A35-2D0ED0275DE2}" name="2021" dataDxfId="31" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{1B444E7A-FFC9-6B49-91BB-1031C0708A5E}" name="Balance Sheet" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{D3F71987-10EB-C24C-A913-E3218D5AFC35}" name="2024" dataDxfId="60" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{72BC2940-218A-304A-AAD0-A2F5E78D3BBC}" name="2023" dataDxfId="59" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{86C26E68-D535-F24E-9210-117B8E1D52B4}" name="2022" dataDxfId="58" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{0E7F4F14-D42E-7647-9A35-2D0ED0275DE2}" name="2021" dataDxfId="57" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7167,69 +7022,69 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="74" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="1" operator="lessThan">
       <formula>0.07</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="between">
       <formula>0.07</formula>
       <formula>0.135</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="3" operator="greaterThan">
       <formula>0.17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:K6 L6 I11:L11 I15">
-    <cfRule type="containsText" dxfId="71" priority="18" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="53" priority="18" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="19" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="52" priority="19" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:L8">
-    <cfRule type="cellIs" dxfId="69" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="11" operator="greaterThan">
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="12" operator="lessThan">
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="13" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:L9">
-    <cfRule type="cellIs" dxfId="66" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="9" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="10" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:L10">
-    <cfRule type="cellIs" dxfId="64" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="4" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="45" priority="7" operator="between">
       <formula>0.8</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="8" operator="lessThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:L14">
-    <cfRule type="containsText" dxfId="61" priority="16" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="43" priority="16" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="17" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="42" priority="17" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:L14">
-    <cfRule type="cellIs" dxfId="59" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="5" operator="lessThan">
       <formula>0.23</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="greaterThan">
       <formula>0.23</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7285,20 +7140,20 @@
     </row>
     <row r="2" spans="1:22" ht="16" thickBot="1">
       <c r="A2" s="36"/>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="93" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="93" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="93" t="s">
         <v>173</v>
-      </c>
-      <c r="E2" s="84" t="s">
-        <v>174</v>
-      </c>
-      <c r="F2" s="84" t="s">
-        <v>175</v>
       </c>
       <c r="G2" s="36"/>
       <c r="H2" s="75" t="s">
@@ -7324,13 +7179,13 @@
     </row>
     <row r="3" spans="1:22" ht="25">
       <c r="A3" s="36"/>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="97"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="96"/>
       <c r="G3" s="36"/>
       <c r="H3" s="36"/>
       <c r="I3" s="36"/>
@@ -7350,13 +7205,13 @@
     </row>
     <row r="4" spans="1:22" ht="18">
       <c r="A4" s="36"/>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="101"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="99"/>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
       <c r="I4" s="36"/>
@@ -7376,13 +7231,13 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="36"/>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="95"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="101"/>
       <c r="G5" s="36"/>
       <c r="H5" s="36"/>
       <c r="I5" s="36"/>
@@ -7402,13 +7257,13 @@
     </row>
     <row r="6" spans="1:22" ht="25">
       <c r="A6" s="36"/>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="97"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="96"/>
       <c r="G6" s="36"/>
       <c r="H6" s="36"/>
       <c r="I6" s="36"/>
@@ -7428,13 +7283,13 @@
     </row>
     <row r="7" spans="1:22" ht="25">
       <c r="A7" s="36"/>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="97"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="96"/>
       <c r="G7" s="36"/>
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
@@ -7454,13 +7309,13 @@
     </row>
     <row r="8" spans="1:22" ht="25">
       <c r="A8" s="36"/>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="95"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="101"/>
       <c r="G8" s="36"/>
       <c r="H8" s="36"/>
       <c r="I8" s="36"/>
@@ -7480,13 +7335,13 @@
     </row>
     <row r="9" spans="1:22" ht="25">
       <c r="A9" s="36"/>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="97"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="96"/>
       <c r="G9" s="36"/>
       <c r="H9" s="36"/>
       <c r="I9" s="36"/>
@@ -7506,13 +7361,13 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="36"/>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="95"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="101"/>
       <c r="G10" s="36"/>
       <c r="H10" s="36"/>
       <c r="I10" s="36"/>
@@ -7532,13 +7387,13 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="36"/>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="94"/>
-      <c r="F11" s="95"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="101"/>
       <c r="G11" s="36"/>
       <c r="H11" s="36"/>
       <c r="I11" s="36"/>
@@ -7558,13 +7413,13 @@
     </row>
     <row r="12" spans="1:22" ht="25">
       <c r="A12" s="36"/>
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="97"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="96"/>
       <c r="G12" s="36"/>
       <c r="H12" s="36"/>
       <c r="I12" s="36"/>
@@ -7584,13 +7439,13 @@
     </row>
     <row r="13" spans="1:22" ht="25">
       <c r="A13" s="36"/>
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="97"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="96"/>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
       <c r="I13" s="36"/>
@@ -7610,13 +7465,13 @@
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="36"/>
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="104"/>
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
       <c r="I14" s="36"/>
@@ -7636,13 +7491,13 @@
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="36"/>
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="95"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="101"/>
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
       <c r="I15" s="36"/>
@@ -7662,13 +7517,13 @@
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="36"/>
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="103"/>
+      <c r="F16" s="104"/>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
@@ -7686,15 +7541,15 @@
       <c r="U16" s="36"/>
       <c r="V16" s="36"/>
     </row>
-    <row r="17" spans="1:22" ht="18">
+    <row r="17" spans="1:22" ht="19" thickBot="1">
       <c r="A17" s="36"/>
-      <c r="B17" s="91" t="s">
+      <c r="B17" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="99"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="107"/>
       <c r="G17" s="36"/>
       <c r="H17" s="36"/>
       <c r="I17" s="36"/>
@@ -8956,25 +8811,24 @@
       <c r="V59" s="36"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="28" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="19" operator="greaterThan">
+      <formula>0.17</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="18" operator="between">
       <formula>0</formula>
       <formula>0.135</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="19" operator="greaterThan">
-      <formula>0.17</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:E23 F23 C28:F28 C32">
-    <cfRule type="containsText" dxfId="25" priority="32" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="36" priority="33" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",C21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="32" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",C21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="33" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",C21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:F3">
@@ -9134,70 +8988,67 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:F24">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="between">
       <formula>0.2</formula>
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="lessThan">
       <formula>0.2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="greaterThan">
+      <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:F25">
-    <cfRule type="cellIs" dxfId="20" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="27" operator="greaterThan">
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="28" operator="between">
       <formula>0.1</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:F26">
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="25" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="26" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:F27">
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="between">
       <formula>0.8</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="lessThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:F31">
-    <cfRule type="containsText" dxfId="12" priority="30" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="23" priority="30" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",C30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="31" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="22" priority="31" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:F31">
-    <cfRule type="cellIs" dxfId="10" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="lessThan">
       <formula>0.23</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="greaterThan">
       <formula>0.23</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -9252,19 +9103,19 @@
     </row>
     <row r="2" spans="1:22" ht="16" thickBot="1">
       <c r="A2" s="36"/>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="E2" s="90" t="s">
+      <c r="E2" s="89" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="90" t="s">
+      <c r="F2" s="89" t="s">
         <v>171</v>
       </c>
       <c r="G2" s="36"/>
@@ -9291,19 +9142,19 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="36"/>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="85">
+      <c r="C3" s="84">
         <v>5282000</v>
       </c>
-      <c r="D3" s="85">
+      <c r="D3" s="84">
         <v>5159000</v>
       </c>
-      <c r="E3" s="85">
+      <c r="E3" s="84">
         <v>2605000</v>
       </c>
-      <c r="F3" s="86">
+      <c r="F3" s="85">
         <v>1826000</v>
       </c>
       <c r="G3" s="36"/>
@@ -9325,19 +9176,19 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="36"/>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="85">
+      <c r="C4" s="84">
         <v>5260000</v>
       </c>
-      <c r="D4" s="85">
+      <c r="D4" s="84">
         <v>4845000</v>
       </c>
-      <c r="E4" s="85">
+      <c r="E4" s="84">
         <v>3607000</v>
       </c>
-      <c r="F4" s="86">
+      <c r="F4" s="85">
         <v>2856000</v>
       </c>
       <c r="G4" s="36"/>
@@ -9359,19 +9210,19 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="36"/>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="85">
+      <c r="C5" s="84">
         <v>5542000</v>
       </c>
-      <c r="D5" s="85">
+      <c r="D5" s="84">
         <v>6048000</v>
       </c>
-      <c r="E5" s="85">
+      <c r="E5" s="84">
         <v>6688000</v>
       </c>
-      <c r="F5" s="86">
+      <c r="F5" s="85">
         <v>6930000</v>
       </c>
       <c r="G5" s="36"/>
@@ -9393,19 +9244,19 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="36"/>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="85">
+      <c r="C6" s="84">
         <v>65728000</v>
       </c>
-      <c r="D6" s="85">
+      <c r="D6" s="84">
         <v>41182000</v>
       </c>
-      <c r="E6" s="85">
+      <c r="E6" s="84">
         <v>44187000</v>
       </c>
-      <c r="F6" s="86">
+      <c r="F6" s="85">
         <v>28791000</v>
       </c>
       <c r="G6" s="36"/>
@@ -9427,19 +9278,19 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="36"/>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="85">
+      <c r="C7" s="84">
         <v>10631000</v>
       </c>
-      <c r="D7" s="85">
+      <c r="D7" s="84">
         <v>6563000</v>
       </c>
-      <c r="E7" s="85">
+      <c r="E7" s="84">
         <v>4335000</v>
       </c>
-      <c r="F7" s="86">
+      <c r="F7" s="85">
         <v>3925000</v>
       </c>
       <c r="G7" s="36"/>
@@ -9461,19 +9312,19 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="36"/>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="85">
+      <c r="C8" s="84">
         <v>12119000</v>
       </c>
-      <c r="D8" s="85">
+      <c r="D8" s="84">
         <v>12518000</v>
       </c>
-      <c r="E8" s="85">
+      <c r="E8" s="84">
         <v>13240000</v>
       </c>
-      <c r="F8" s="86">
+      <c r="F8" s="85">
         <v>7973000</v>
       </c>
       <c r="G8" s="36"/>
@@ -9495,19 +9346,19 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="36"/>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="84">
         <v>22750000</v>
       </c>
-      <c r="D9" s="85">
+      <c r="D9" s="84">
         <v>19081000</v>
       </c>
-      <c r="E9" s="85">
+      <c r="E9" s="84">
         <v>17575000</v>
       </c>
-      <c r="F9" s="86">
+      <c r="F9" s="85">
         <v>11898000</v>
       </c>
       <c r="G9" s="36"/>
@@ -9529,19 +9380,19 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="36"/>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="85">
+      <c r="C10" s="84">
         <v>0</v>
       </c>
-      <c r="D10" s="85">
+      <c r="D10" s="84">
         <v>0</v>
       </c>
-      <c r="E10" s="85">
+      <c r="E10" s="84">
         <v>0</v>
       </c>
-      <c r="F10" s="86">
+      <c r="F10" s="85">
         <v>10756000</v>
       </c>
       <c r="G10" s="36"/>
@@ -9563,19 +9414,19 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="36"/>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="84">
         <v>0</v>
       </c>
-      <c r="D11" s="85">
+      <c r="D11" s="84">
         <v>0</v>
       </c>
-      <c r="E11" s="85">
+      <c r="E11" s="84">
         <v>0</v>
       </c>
-      <c r="F11" s="86">
+      <c r="F11" s="85">
         <v>0</v>
       </c>
       <c r="G11" s="36"/>
@@ -9597,19 +9448,19 @@
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="36"/>
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="85">
+      <c r="C12" s="84">
         <v>29817000</v>
       </c>
-      <c r="D12" s="85">
+      <c r="D12" s="84">
         <v>10171000</v>
       </c>
-      <c r="E12" s="85">
+      <c r="E12" s="84">
         <v>16235000</v>
       </c>
-      <c r="F12" s="86">
+      <c r="F12" s="85">
         <v>18908000</v>
       </c>
       <c r="G12" s="36"/>
@@ -9631,19 +9482,19 @@
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="36"/>
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="85">
+      <c r="C13" s="84">
         <v>42978000</v>
       </c>
-      <c r="D13" s="85">
+      <c r="D13" s="84">
         <v>22101000</v>
       </c>
-      <c r="E13" s="85">
+      <c r="E13" s="84">
         <v>26612000</v>
       </c>
-      <c r="F13" s="86">
+      <c r="F13" s="85">
         <v>16893000</v>
       </c>
       <c r="G13" s="36"/>
@@ -9665,13 +9516,13 @@
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="36"/>
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
       <c r="I14" s="36"/>
@@ -9691,19 +9542,19 @@
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="36"/>
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="85">
+      <c r="C15" s="84">
         <v>8675000</v>
       </c>
-      <c r="D15" s="85">
+      <c r="D15" s="84">
         <v>7339000</v>
       </c>
-      <c r="E15" s="85">
+      <c r="E15" s="84">
         <v>5268000</v>
       </c>
-      <c r="F15" s="86">
+      <c r="F15" s="85">
         <v>3924000</v>
       </c>
       <c r="G15" s="36"/>
@@ -9725,13 +9576,13 @@
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="36"/>
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
@@ -9751,19 +9602,19 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="36"/>
-      <c r="B17" s="91" t="s">
+      <c r="B17" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="87">
+      <c r="C17" s="86">
         <v>28090000</v>
       </c>
-      <c r="D17" s="87">
+      <c r="D17" s="86">
         <v>5641000</v>
       </c>
-      <c r="E17" s="87">
+      <c r="E17" s="86">
         <v>9108000</v>
       </c>
-      <c r="F17" s="88">
+      <c r="F17" s="87">
         <v>5822000</v>
       </c>
       <c r="G17" s="36"/>
@@ -11029,23 +10880,23 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="57" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
+      <formula>0.17</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="between">
       <formula>0</formula>
       <formula>0.135</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="19" operator="greaterThan">
-      <formula>0.17</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:E23 F23 C28:F28 C32">
-    <cfRule type="containsText" dxfId="54" priority="32" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="16" priority="33" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",C21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="32" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",C21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="33" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",C21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:F3">
@@ -11205,62 +11056,62 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:F24">
-    <cfRule type="cellIs" dxfId="52" priority="1" operator="greaterThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="between">
       <formula>0.2</formula>
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
       <formula>0.2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
+      <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:F25">
-    <cfRule type="cellIs" dxfId="49" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="27" operator="greaterThan">
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="28" operator="between">
       <formula>0.1</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="29" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:F26">
-    <cfRule type="cellIs" dxfId="46" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="25" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="26" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:F27">
-    <cfRule type="cellIs" dxfId="44" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="20" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="23" operator="between">
       <formula>0.8</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="24" operator="lessThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:F31">
-    <cfRule type="containsText" dxfId="41" priority="30" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="3" priority="30" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",C30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="31" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="2" priority="31" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:F31">
-    <cfRule type="cellIs" dxfId="39" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="21" operator="lessThan">
       <formula>0.23</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="22" operator="greaterThan">
       <formula>0.23</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
feat: auto resize column
</commit_message>
<xml_diff>
--- a/input/TICKER_TEMPLATE.xlsx
+++ b/input/TICKER_TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvuolo/Documents/GitHub/dca-2k24/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C5B331-6B71-1C46-9922-8B51F4634EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0CB71F-1C2E-C648-A862-F53C3F3C7023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7620" yWindow="500" windowWidth="40860" windowHeight="28300" activeTab="1" xr2:uid="{372CD787-09C0-4BD9-A6AB-A0065DACB93A}"/>
   </bookViews>
@@ -459,12 +459,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,15 +534,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color rgb="FF0E0E0E"/>
-      <name val=".SF NS"/>
-    </font>
-    <font>
       <sz val="14"/>
-      <color rgb="FF232A31"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -963,7 +957,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1070,23 +1064,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="9" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="9" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="9" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="9" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="9" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="9" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1630,14 +1620,14 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>13</v>
       </c>
@@ -1648,7 +1638,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1659,7 +1649,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1670,7 +1660,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1681,7 +1671,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1692,7 +1682,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1703,7 +1693,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1714,7 +1704,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1725,7 +1715,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1736,7 +1726,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1747,7 +1737,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1758,7 +1748,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1769,13 +1759,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="24">
         <f>SUM(B2:B12)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
         <v>64</v>
       </c>
@@ -1792,7 +1782,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1811,7 +1801,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
         <v>66</v>
       </c>
@@ -1830,7 +1820,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
         <v>67</v>
       </c>
@@ -1849,7 +1839,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G18" s="43">
         <v>3</v>
       </c>
@@ -1865,7 +1855,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="29" t="s">
         <v>68</v>
       </c>
@@ -1884,7 +1874,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
         <v>16</v>
       </c>
@@ -1903,7 +1893,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
         <v>69</v>
       </c>
@@ -1925,7 +1915,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
         <v>70</v>
       </c>
@@ -1947,7 +1937,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
         <v>71</v>
       </c>
@@ -1969,7 +1959,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
         <v>85</v>
       </c>
@@ -1989,7 +1979,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
         <v>72</v>
       </c>
@@ -2011,7 +2001,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
         <v>73</v>
       </c>
@@ -2033,7 +2023,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
         <v>74</v>
       </c>
@@ -2054,13 +2044,13 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
         <v>86</v>
       </c>
       <c r="B28" s="34"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
         <v>75</v>
       </c>
@@ -2068,7 +2058,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
         <v>76</v>
       </c>
@@ -2076,16 +2066,16 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B31" s="34"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="27" t="s">
         <v>87</v>
       </c>
       <c r="B32" s="34"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="30" t="s">
         <v>77</v>
       </c>
@@ -2093,7 +2083,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
         <v>78</v>
       </c>
@@ -2101,7 +2091,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="30" t="s">
         <v>79</v>
       </c>
@@ -2109,16 +2099,16 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B36" s="34"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
         <v>88</v>
       </c>
       <c r="B37" s="34"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="30" t="s">
         <v>80</v>
       </c>
@@ -2126,7 +2116,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
         <v>81</v>
       </c>
@@ -2134,7 +2124,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="30" t="s">
         <v>82</v>
       </c>
@@ -2142,16 +2132,16 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" s="34"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="27" t="s">
         <v>89</v>
       </c>
       <c r="B42" s="34"/>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="30" t="s">
         <v>83</v>
       </c>
@@ -2159,7 +2149,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="30" t="s">
         <v>84</v>
       </c>
@@ -2167,7 +2157,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="30"/>
     </row>
   </sheetData>
@@ -2181,10 +2171,10 @@
   <dimension ref="A1:V59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="214" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.1640625" customWidth="1"/>
     <col min="2" max="2" width="35.6640625" customWidth="1"/>
@@ -2198,7 +2188,7 @@
     <col min="22" max="22" width="140.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="10.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:22" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -2222,7 +2212,7 @@
       <c r="U1" s="20"/>
       <c r="V1" s="20"/>
     </row>
-    <row r="2" spans="1:22" ht="16" thickBot="1">
+    <row r="2" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="47" t="s">
         <v>38</v>
@@ -2261,15 +2251,15 @@
       <c r="U2" s="20"/>
       <c r="V2" s="20"/>
     </row>
-    <row r="3" spans="1:22" ht="25">
+    <row r="3" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="54"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
@@ -2287,9 +2277,9 @@
       <c r="U3" s="20"/>
       <c r="V3" s="20"/>
     </row>
-    <row r="4" spans="1:22" ht="18">
+    <row r="4" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="50" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="53"/>
@@ -2313,15 +2303,15 @@
       <c r="U4" s="20"/>
       <c r="V4" s="20"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="54"/>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -2339,15 +2329,15 @@
       <c r="U5" s="20"/>
       <c r="V5" s="20"/>
     </row>
-    <row r="6" spans="1:22" ht="25">
+    <row r="6" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="51"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="54"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
@@ -2365,15 +2355,15 @@
       <c r="U6" s="20"/>
       <c r="V6" s="20"/>
     </row>
-    <row r="7" spans="1:22" ht="25">
+    <row r="7" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="51"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="54"/>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
@@ -2391,15 +2381,15 @@
       <c r="U7" s="20"/>
       <c r="V7" s="20"/>
     </row>
-    <row r="8" spans="1:22" ht="25">
+    <row r="8" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="56"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="54"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
@@ -2417,15 +2407,15 @@
       <c r="U8" s="20"/>
       <c r="V8" s="20"/>
     </row>
-    <row r="9" spans="1:22" ht="25">
+    <row r="9" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="51"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
@@ -2443,15 +2433,15 @@
       <c r="U9" s="20"/>
       <c r="V9" s="20"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
@@ -2469,15 +2459,15 @@
       <c r="U10" s="20"/>
       <c r="V10" s="20"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="56"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
@@ -2495,15 +2485,15 @@
       <c r="U11" s="20"/>
       <c r="V11" s="20"/>
     </row>
-    <row r="12" spans="1:22" ht="25">
+    <row r="12" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="51"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="54"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
@@ -2521,15 +2511,15 @@
       <c r="U12" s="20"/>
       <c r="V12" s="20"/>
     </row>
-    <row r="13" spans="1:22" ht="25">
+    <row r="13" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="51"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="54"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -2547,15 +2537,15 @@
       <c r="U13" s="20"/>
       <c r="V13" s="20"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="59"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
@@ -2573,15 +2563,15 @@
       <c r="U14" s="20"/>
       <c r="V14" s="20"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="54"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
@@ -2599,15 +2589,15 @@
       <c r="U15" s="20"/>
       <c r="V15" s="20"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="59"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
       <c r="I16" s="20"/>
@@ -2625,15 +2615,15 @@
       <c r="U16" s="20"/>
       <c r="V16" s="20"/>
     </row>
-    <row r="17" spans="1:22" ht="19" thickBot="1">
+    <row r="17" spans="1:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="62"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
@@ -2651,7 +2641,7 @@
       <c r="U17" s="20"/>
       <c r="V17" s="20"/>
     </row>
-    <row r="18" spans="1:22" ht="16" thickBot="1">
+    <row r="18" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
@@ -2675,7 +2665,7 @@
       <c r="U18" s="20"/>
       <c r="V18" s="20"/>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="22" t="s">
         <v>13</v>
@@ -2711,7 +2701,7 @@
       <c r="U19" s="20"/>
       <c r="V19" s="20"/>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="15" t="s">
         <v>14</v>
@@ -2739,7 +2729,7 @@
       <c r="U20" s="20"/>
       <c r="V20" s="20"/>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="16" t="s">
         <v>25</v>
@@ -2779,7 +2769,7 @@
       <c r="U21" s="20"/>
       <c r="V21" s="20"/>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="16" t="s">
         <v>26</v>
@@ -2819,7 +2809,7 @@
       <c r="U22" s="20"/>
       <c r="V22" s="20"/>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="15" t="s">
         <v>15</v>
@@ -2862,7 +2852,7 @@
       <c r="U23" s="20"/>
       <c r="V23" s="20"/>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="15" t="s">
         <v>16</v>
@@ -2908,7 +2898,7 @@
       <c r="U24" s="20"/>
       <c r="V24" s="20"/>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="15" t="s">
         <v>17</v>
@@ -2954,7 +2944,7 @@
       <c r="U25" s="20"/>
       <c r="V25" s="20"/>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="20"/>
       <c r="B26" s="15" t="s">
         <v>18</v>
@@ -3000,7 +2990,7 @@
       <c r="U26" s="20"/>
       <c r="V26" s="20"/>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
       <c r="B27" s="15" t="s">
         <v>19</v>
@@ -3046,7 +3036,7 @@
       <c r="U27" s="20"/>
       <c r="V27" s="20"/>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
       <c r="B28" s="15" t="s">
         <v>20</v>
@@ -3089,7 +3079,7 @@
       <c r="U28" s="20"/>
       <c r="V28" s="20"/>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="20"/>
       <c r="B29" s="15" t="s">
         <v>21</v>
@@ -3123,7 +3113,7 @@
       <c r="U29" s="20"/>
       <c r="V29" s="20"/>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="20"/>
       <c r="B30" s="15" t="s">
         <v>22</v>
@@ -3166,7 +3156,7 @@
       <c r="U30" s="20"/>
       <c r="V30" s="20"/>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="20"/>
       <c r="B31" s="15" t="s">
         <v>23</v>
@@ -3212,7 +3202,7 @@
       <c r="U31" s="20"/>
       <c r="V31" s="20"/>
     </row>
-    <row r="32" spans="1:22" ht="16" thickBot="1">
+    <row r="32" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
       <c r="B32" s="9" t="s">
         <v>24</v>
@@ -3246,7 +3236,7 @@
       <c r="U32" s="20"/>
       <c r="V32" s="20"/>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
@@ -3270,7 +3260,7 @@
       <c r="U33" s="20"/>
       <c r="V33" s="20"/>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
@@ -3294,7 +3284,7 @@
       <c r="U34" s="20"/>
       <c r="V34" s="20"/>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
@@ -3318,7 +3308,7 @@
       <c r="U35" s="20"/>
       <c r="V35" s="20"/>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -3342,7 +3332,7 @@
       <c r="U36" s="20"/>
       <c r="V36" s="20"/>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
@@ -3366,7 +3356,7 @@
       <c r="U37" s="20"/>
       <c r="V37" s="20"/>
     </row>
-    <row r="38" spans="1:22">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="20"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
@@ -3390,7 +3380,7 @@
       <c r="U38" s="20"/>
       <c r="V38" s="20"/>
     </row>
-    <row r="39" spans="1:22">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
@@ -3414,7 +3404,7 @@
       <c r="U39" s="20"/>
       <c r="V39" s="20"/>
     </row>
-    <row r="40" spans="1:22">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="20"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
@@ -3438,7 +3428,7 @@
       <c r="U40" s="20"/>
       <c r="V40" s="20"/>
     </row>
-    <row r="41" spans="1:22">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
@@ -3462,7 +3452,7 @@
       <c r="U41" s="20"/>
       <c r="V41" s="20"/>
     </row>
-    <row r="42" spans="1:22">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="20"/>
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
@@ -3486,7 +3476,7 @@
       <c r="U42" s="20"/>
       <c r="V42" s="20"/>
     </row>
-    <row r="43" spans="1:22">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
@@ -3510,7 +3500,7 @@
       <c r="U43" s="20"/>
       <c r="V43" s="20"/>
     </row>
-    <row r="44" spans="1:22">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="20"/>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
@@ -3534,7 +3524,7 @@
       <c r="U44" s="20"/>
       <c r="V44" s="20"/>
     </row>
-    <row r="45" spans="1:22">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" s="20"/>
       <c r="B45" s="20"/>
       <c r="C45" s="20"/>
@@ -3558,7 +3548,7 @@
       <c r="U45" s="20"/>
       <c r="V45" s="20"/>
     </row>
-    <row r="46" spans="1:22">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="20"/>
       <c r="B46" s="20"/>
       <c r="C46" s="20"/>
@@ -3582,7 +3572,7 @@
       <c r="U46" s="20"/>
       <c r="V46" s="20"/>
     </row>
-    <row r="47" spans="1:22">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="20"/>
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
@@ -3606,7 +3596,7 @@
       <c r="U47" s="20"/>
       <c r="V47" s="20"/>
     </row>
-    <row r="48" spans="1:22">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="20"/>
       <c r="B48" s="20"/>
       <c r="C48" s="20"/>
@@ -3630,7 +3620,7 @@
       <c r="U48" s="20"/>
       <c r="V48" s="20"/>
     </row>
-    <row r="49" spans="1:22">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="20"/>
       <c r="B49" s="20"/>
       <c r="C49" s="20"/>
@@ -3654,7 +3644,7 @@
       <c r="U49" s="20"/>
       <c r="V49" s="20"/>
     </row>
-    <row r="50" spans="1:22">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="20"/>
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
@@ -3678,7 +3668,7 @@
       <c r="U50" s="20"/>
       <c r="V50" s="20"/>
     </row>
-    <row r="51" spans="1:22">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="20"/>
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
@@ -3702,7 +3692,7 @@
       <c r="U51" s="20"/>
       <c r="V51" s="20"/>
     </row>
-    <row r="52" spans="1:22">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="20"/>
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
@@ -3726,7 +3716,7 @@
       <c r="U52" s="20"/>
       <c r="V52" s="20"/>
     </row>
-    <row r="53" spans="1:22">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
@@ -3750,7 +3740,7 @@
       <c r="U53" s="20"/>
       <c r="V53" s="20"/>
     </row>
-    <row r="54" spans="1:22">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
@@ -3774,7 +3764,7 @@
       <c r="U54" s="20"/>
       <c r="V54" s="20"/>
     </row>
-    <row r="55" spans="1:22">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
@@ -3798,7 +3788,7 @@
       <c r="U55" s="20"/>
       <c r="V55" s="20"/>
     </row>
-    <row r="56" spans="1:22">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
       <c r="C56" s="20"/>
@@ -3822,7 +3812,7 @@
       <c r="U56" s="20"/>
       <c r="V56" s="20"/>
     </row>
-    <row r="57" spans="1:22">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="C57" s="20"/>
@@ -3846,7 +3836,7 @@
       <c r="U57" s="20"/>
       <c r="V57" s="20"/>
     </row>
-    <row r="58" spans="1:22">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
@@ -3870,7 +3860,7 @@
       <c r="U58" s="20"/>
       <c r="V58" s="20"/>
     </row>
-    <row r="59" spans="1:22">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="20"/>
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>

</xml_diff>

<commit_message>
style: update template styling
</commit_message>
<xml_diff>
--- a/input/TICKER_TEMPLATE.xlsx
+++ b/input/TICKER_TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvuolo/Documents/GitHub/dca-2k24/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0CB71F-1C2E-C648-A862-F53C3F3C7023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAA1F08-8E76-BC40-BE41-24AD919088CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7620" yWindow="500" windowWidth="40860" windowHeight="28300" activeTab="1" xr2:uid="{372CD787-09C0-4BD9-A6AB-A0065DACB93A}"/>
   </bookViews>
@@ -459,9 +459,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -962,11 +963,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -975,10 +976,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1071,12 +1072,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="9" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="9" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="9" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="9" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="9" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="9" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="9" fillId="4" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="9" fillId="2" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="9" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="9" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="9" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>

</xml_diff>

<commit_message>
feat: structured summary page
</commit_message>
<xml_diff>
--- a/input/TICKER_TEMPLATE.xlsx
+++ b/input/TICKER_TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvuolo/Documents/GitHub/dca-2k24/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A36155-19C0-F544-A3FB-6F0C2AD38565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BB2B95-77FE-6F44-B427-DF46E02A3811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7620" yWindow="500" windowWidth="40860" windowHeight="28300" xr2:uid="{372CD787-09C0-4BD9-A6AB-A0065DACB93A}"/>
   </bookViews>
@@ -459,7 +459,7 @@
     <t>Ticker</t>
   </si>
   <si>
-    <t>Score Percent</t>
+    <t>Score (%)</t>
   </si>
 </sst>
 </file>
@@ -965,7 +965,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1085,15 +1085,29 @@
     <xf numFmtId="41" fontId="9" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="9" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="9" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1224,16 +1238,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1249,6 +1253,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1279,16 +1303,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1635,47 +1649,50 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="265" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="66" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="63" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="60" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
+      <c r="B1" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="61"/>
+    </row>
+    <row r="2" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="64"/>
+      <c r="B2" s="62"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="59"/>
-      <c r="B3" s="59"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="59"/>
-      <c r="B4" s="59"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="62"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="59"/>
-      <c r="B5" s="59"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="62"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="59"/>
-      <c r="B6" s="59"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="62"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="59"/>
-      <c r="B7" s="59"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3956,20 +3973,20 @@
     <cfRule type="cellIs" dxfId="19" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
-      <formula>0.17</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="between">
       <formula>0</formula>
       <formula>0.135</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="greaterThan">
+      <formula>0.17</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:E23 F23 C28:F28 C32">
-    <cfRule type="containsText" dxfId="16" priority="33" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="16" priority="32" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",C21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="33" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",C21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="32" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",C21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:F3">
@@ -4129,15 +4146,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:F24">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="between">
       <formula>0.2</formula>
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
       <formula>0.2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
-      <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:F25">

</xml_diff>

<commit_message>
feat: back to summary selector
</commit_message>
<xml_diff>
--- a/input/TICKER_TEMPLATE.xlsx
+++ b/input/TICKER_TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvuolo/Documents/GitHub/dca-2k24/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BB2B95-77FE-6F44-B427-DF46E02A3811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49236BBF-989D-7247-8DC1-79057162A805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="500" windowWidth="40860" windowHeight="28300" xr2:uid="{372CD787-09C0-4BD9-A6AB-A0065DACB93A}"/>
+    <workbookView xWindow="7620" yWindow="500" windowWidth="40860" windowHeight="28300" activeTab="2" xr2:uid="{372CD787-09C0-4BD9-A6AB-A0065DACB93A}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="107">
   <si>
     <t>inventory</t>
   </si>
@@ -461,6 +461,9 @@
   <si>
     <t>Score (%)</t>
   </si>
+  <si>
+    <t>&lt;- Back to Summary Sheet</t>
+  </si>
 </sst>
 </file>
 
@@ -471,7 +474,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,6 +550,14 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -960,12 +971,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1085,9 +1097,6 @@
     <xf numFmtId="41" fontId="9" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="9" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="9" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1100,18 +1109,19 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -1238,6 +1248,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1253,26 +1273,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1303,6 +1303,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1648,47 +1658,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7576354F-272E-804C-9155-1CE76271BB53}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView zoomScale="265" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="66" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="63" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="63" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="60" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64"/>
-      <c r="B2" s="62"/>
+    <row r="2" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="63"/>
+      <c r="B2" s="61"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="62"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="61"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="62"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="61"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
-      <c r="B5" s="62"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="61"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="65"/>
-      <c r="B6" s="62"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="61"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="65"/>
-      <c r="B7" s="62"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2254,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8882183-2D9A-6A47-ABB3-41EA243B3A4E}">
   <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView zoomScale="214" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="214" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2272,9 +2280,11 @@
     <col min="22" max="22" width="140.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
+      <c r="B1" s="65" t="s">
+        <v>106</v>
+      </c>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
@@ -3973,20 +3983,20 @@
     <cfRule type="cellIs" dxfId="19" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
+      <formula>0.17</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="between">
       <formula>0</formula>
       <formula>0.135</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="greaterThan">
-      <formula>0.17</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:E23 F23 C28:F28 C32">
-    <cfRule type="containsText" dxfId="16" priority="32" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="16" priority="33" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",C21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="32" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",C21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="33" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",C21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:F3">
@@ -4146,15 +4156,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:F24">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="between">
       <formula>0.2</formula>
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
       <formula>0.2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
+      <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:F25">
@@ -4205,6 +4215,9 @@
       <formula>0.23</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B1" location="Summary!A1" display="&lt;- Back to Summary Sheet" xr:uid="{885B2C39-0F04-2344-A640-6A0F99222F47}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>